<commit_message>
Add title to new column
</commit_message>
<xml_diff>
--- a/inventory_with_total_value.xlsx
+++ b/inventory_with_total_value.xlsx
@@ -370,6 +370,11 @@
           <t>Supplier</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Total Inventory Value</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">

</xml_diff>